<commit_message>
Add updated excel sheet
</commit_message>
<xml_diff>
--- a/PHP Server/Microprocessor_Section_C.xlsx
+++ b/PHP Server/Microprocessor_Section_C.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saqibur\Desktop\Student-Attendance-Using-ESP8266\PHP Server\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814FCB63-1C6E-49B2-AF50-453B839A23A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -41,16 +46,7 @@
     <t>Fahim</t>
   </si>
   <si>
-    <t>4d:fd:dc:16:c9:f1</t>
-  </si>
-  <si>
-    <t>17-00002-1</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>81:4a:1d:03:73:54</t>
+    <t>24:18:1d:1:a8:7d</t>
   </si>
   <si>
     <t>17-00003-1</t>
@@ -59,7 +55,7 @@
     <t>Tanmoy</t>
   </si>
   <si>
-    <t>45:4a:1d:03:73:53</t>
+    <t>94:87:e0:5a:6c:31</t>
   </si>
   <si>
     <t>17-00004-1</t>
@@ -68,7 +64,7 @@
     <t>Sachi</t>
   </si>
   <si>
-    <t>c4:4b:1d:03:73:55</t>
+    <t>20:f4:78:f1:51:82</t>
   </si>
   <si>
     <t>17-00005-1</t>
@@ -77,7 +73,7 @@
     <t>Priya</t>
   </si>
   <si>
-    <t>b4:4a:1d:03:73:56</t>
+    <t>a4:12:32:ea:f9:3</t>
   </si>
   <si>
     <t>17-00006-1</t>
@@ -86,7 +82,7 @@
     <t>Sahil</t>
   </si>
   <si>
-    <t>84:4a:1d:03:73:57</t>
+    <t>bc:e1:43:7e:a9:a4</t>
   </si>
   <si>
     <t>17-00007-1</t>
@@ -95,7 +91,7 @@
     <t>Tasnim</t>
   </si>
   <si>
-    <t>4d:fd:dc:16:c9:f7</t>
+    <t>XX:XX:XX:XX:Xx</t>
   </si>
   <si>
     <t>17-00008-1</t>
@@ -110,14 +106,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -128,34 +119,43 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="14" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -445,28 +445,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="true" style="0"/>
-    <col min="2" max="2" width="19.28515625" customWidth="true" style="0"/>
-    <col min="3" max="3" width="13.7109375" customWidth="true" style="0"/>
-    <col min="4" max="4" width="30.28515625" customWidth="true" style="0"/>
-    <col min="5" max="5" width="11.5703125" customWidth="true" style="0"/>
-    <col min="6" max="6" width="13.85546875" customWidth="true" style="0"/>
-    <col min="7" max="7" width="13.28515625" customWidth="true" style="0"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,7 +492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -524,7 +521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -538,11 +535,11 @@
         <v>11</v>
       </c>
       <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
@@ -553,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -582,7 +579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -596,7 +593,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -611,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -625,7 +622,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -640,7 +637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -654,10 +651,10 @@
         <v>23</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -669,7 +666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -677,13 +674,13 @@
         <v>25</v>
       </c>
       <c r="C8" s="1">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -695,50 +692,11 @@
         <v>1</v>
       </c>
       <c r="I8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>